<commit_message>
jlc pick and place seems to kinda work
</commit_message>
<xml_diff>
--- a/UWB_Anchor/Project Outputs for UWB_Anchor/BOM/Bill of Materials-UWB_Anchor.xlsx
+++ b/UWB_Anchor/Project Outputs for UWB_Anchor/BOM/Bill of Materials-UWB_Anchor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shared\fydp\fydp-anchor-pcb\UWB_Anchor\Project Outputs for UWB_Anchor\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{742D066C-F9D3-4416-9CA6-8137AD1DF476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6F149F0-6648-4D4B-97B9-603E1307A3D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="255" windowWidth="21330" windowHeight="11295" xr2:uid="{E814AF46-E2DE-4C0E-9B83-5ADA50B2FBA9}"/>
+    <workbookView xWindow="7470" yWindow="255" windowWidth="21330" windowHeight="11295" xr2:uid="{F8159479-DAB3-4494-AE7C-E12A976416C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-UWB_Anchor" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
   <si>
     <t>Designator</t>
   </si>
@@ -464,6 +464,9 @@
     <t>TS-1187A-B-A-B</t>
   </si>
   <si>
+    <t>C318884</t>
+  </si>
+  <si>
     <t>U1</t>
   </si>
   <si>
@@ -518,6 +521,9 @@
     <t>Y1</t>
   </si>
   <si>
+    <t>25MHz</t>
+  </si>
+  <si>
     <t>XTAL_TSX-3225_25.0000MF20P-C0</t>
   </si>
   <si>
@@ -525,6 +531,9 @@
   </si>
   <si>
     <t>X322525MOB4SI</t>
+  </si>
+  <si>
+    <t>C9006</t>
   </si>
 </sst>
 </file>
@@ -900,7 +909,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D7FE83-75D8-4D0A-ADB4-F46AED6BA42B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{797ADA6B-4804-4354-BE39-EC8619973747}">
   <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1748,7 +1757,7 @@
         <v>13</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H34" s="1">
         <v>2</v>
@@ -1756,23 +1765,23 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
@@ -1780,23 +1789,23 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H36" s="1">
         <v>1</v>
@@ -1804,23 +1813,23 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>152</v>
-      </c>
       <c r="F37" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="H37" s="1">
         <v>1</v>
@@ -1828,23 +1837,23 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D38" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>155</v>
-      </c>
       <c r="F38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H38" s="1">
         <v>1</v>
@@ -1852,23 +1861,25 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B39" s="1"/>
+        <v>159</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="C39" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="F39" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H39" s="1">
         <v>1</v>

</xml_diff>

<commit_message>
final commit before order
</commit_message>
<xml_diff>
--- a/UWB_Anchor/Project Outputs for UWB_Anchor/BOM/Bill of Materials-UWB_Anchor.xlsx
+++ b/UWB_Anchor/Project Outputs for UWB_Anchor/BOM/Bill of Materials-UWB_Anchor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\shared\fydp\fydp-anchor-pcb\UWB_Anchor\Project Outputs for UWB_Anchor\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1FAADA8-9042-4A7C-903A-9077431CFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D668436-132D-4149-BF45-69F8E40B8562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7470" yWindow="255" windowWidth="21330" windowHeight="11295" xr2:uid="{4DB29CFA-0EB5-4687-9999-1F762E3F959C}"/>
+    <workbookView xWindow="7470" yWindow="255" windowWidth="21330" windowHeight="11295" xr2:uid="{904F090F-945D-4602-8B14-C6A403A975AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-UWB_Anchor" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="168">
   <si>
     <t>Designator</t>
   </si>
@@ -227,7 +227,22 @@
     <t>C19666</t>
   </si>
   <si>
-    <t>D1, D3, D4, D5, D6</t>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>FP-SMAJ-MFG</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>BLM21AG121SH1D</t>
+  </si>
+  <si>
+    <t>81-BLM21AG121SH1D</t>
+  </si>
+  <si>
+    <t>D2, D3, D4, D5, D6</t>
   </si>
   <si>
     <t>0805 LED</t>
@@ -242,21 +257,6 @@
     <t>C84256, C2297, C2296</t>
   </si>
   <si>
-    <t>D2</t>
-  </si>
-  <si>
-    <t>FP-SMAJ-MFG</t>
-  </si>
-  <si>
-    <t>Murata Electronics</t>
-  </si>
-  <si>
-    <t>BLM21AG121SH1D</t>
-  </si>
-  <si>
-    <t>81-BLM21AG121SH1D</t>
-  </si>
-  <si>
     <t>F1, F2</t>
   </si>
   <si>
@@ -302,7 +302,7 @@
     <t>HDR1X3</t>
   </si>
   <si>
-    <t>J4, J5, J6, J7, J8</t>
+    <t>J4, J5, J6, J7, J8, J9</t>
   </si>
   <si>
     <t>HDR1X2</t>
@@ -335,7 +335,7 @@
     <t>C236232</t>
   </si>
   <si>
-    <t>R1, R2, R13, R14, R15, R16, R17, R20, R21</t>
+    <t>R1, R2, R15, R16, R17, R18, R19, R22, R23</t>
   </si>
   <si>
     <t>1k</t>
@@ -401,10 +401,19 @@
     <t>C21189</t>
   </si>
   <si>
-    <t>R18, R19, R32</t>
-  </si>
-  <si>
-    <t>R22, R23</t>
+    <t>R13, R14</t>
+  </si>
+  <si>
+    <t>100 / 0.25W</t>
+  </si>
+  <si>
+    <t>RESAD1100W55L680D260</t>
+  </si>
+  <si>
+    <t>R20, R21, R34</t>
+  </si>
+  <si>
+    <t>R24, R25</t>
   </si>
   <si>
     <t>100k</t>
@@ -416,7 +425,7 @@
     <t>C25803</t>
   </si>
   <si>
-    <t>R24</t>
+    <t>R26</t>
   </si>
   <si>
     <t>1M</t>
@@ -428,7 +437,7 @@
     <t>C22935</t>
   </si>
   <si>
-    <t>R25, R26, R28, R29, R30, R31, R33</t>
+    <t>R27, R28, R30, R31, R32, R33, R35</t>
   </si>
   <si>
     <t>10k</t>
@@ -440,7 +449,7 @@
     <t>C25804</t>
   </si>
   <si>
-    <t>R27</t>
+    <t>R29</t>
   </si>
   <si>
     <t>2.4k</t>
@@ -909,8 +918,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F931949-416B-4E3D-8293-C04814A51706}">
-  <dimension ref="A1:H39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5CBABD-3EFC-4A5E-9119-4C6317E92291}">
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1263,9 +1272,7 @@
       <c r="A14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1276,20 +1283,22 @@
         <v>65</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>66</v>
       </c>
       <c r="H14" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
       <c r="C15" s="2" t="s">
         <v>68</v>
       </c>
@@ -1300,13 +1309,13 @@
         <v>70</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>71</v>
       </c>
       <c r="H15" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1342,16 +1351,16 @@
         <v>78</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>34</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H17" s="1">
         <v>1</v>
@@ -1426,7 +1435,7 @@
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -1438,7 +1447,7 @@
         <v>90</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>91</v>
@@ -1612,10 +1621,10 @@
         <v>120</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>44</v>
+        <v>121</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>100</v>
+        <v>122</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>45</v>
@@ -1630,41 +1639,41 @@
         <v>45</v>
       </c>
       <c r="H29" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>122</v>
+        <v>44</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>100</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>101</v>
+        <v>45</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>123</v>
+        <v>45</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>13</v>
+        <v>45</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="H30" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>125</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>126</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>100</v>
@@ -1673,24 +1682,24 @@
         <v>101</v>
       </c>
       <c r="E31" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>128</v>
-      </c>
       <c r="H31" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>129</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>130</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>100</v>
@@ -1699,24 +1708,24 @@
         <v>101</v>
       </c>
       <c r="E32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F32" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>132</v>
-      </c>
       <c r="H32" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>100</v>
@@ -1725,87 +1734,89 @@
         <v>101</v>
       </c>
       <c r="E33" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="H33" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="C34" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="F34" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>141</v>
-      </c>
       <c r="H34" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="F35" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="H35" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="F36" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="H36" s="1">
         <v>1</v>
@@ -1813,23 +1824,23 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>153</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="H37" s="1">
         <v>1</v>
@@ -1850,10 +1861,10 @@
         <v>156</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>13</v>
+        <v>157</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="H38" s="1">
         <v>1</v>
@@ -1861,27 +1872,51 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="E39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="H39" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E39" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="H39" s="1">
+      <c r="D40" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="H40" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>